<commit_message>
Yet another update to excel
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,17 +500,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Relite Finance</t>
+          <t>Wenlambo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7 hours</t>
+          <t xml:space="preserve"> 5 hours</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -530,47 +530,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>420x</t>
+          <t>SafeMusk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 hours</t>
+          <t xml:space="preserve"> 10 hours</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EthereumMax</t>
+          <t>YooShi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t xml:space="preserve"> 13 hours</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -580,37 +580,37 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MoonJuice</t>
+          <t>Rune</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t xml:space="preserve"> 15 hours</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -620,22 +620,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Float Protocol: Float</t>
+          <t>Tiger King</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t xml:space="preserve"> 15 hours</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -644,23 +644,23 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LaunchX</t>
+          <t>GeroWallet</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t xml:space="preserve"> 17 hours</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -670,37 +670,37 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nafter</t>
+          <t>Exohood</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t xml:space="preserve"> 22 hours</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -710,17 +710,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Alaska Inu</t>
+          <t>Relite Finance</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -730,37 +730,37 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Elongate Deluxe</t>
+          <t>Convex Finance</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -770,87 +770,87 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SafeZone</t>
+          <t>420x</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Change Our World</t>
+          <t>EthereumMax</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pinknode</t>
+          <t>Float Protocol: Float</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -860,7 +860,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Avalaunch</t>
+          <t>LaunchX</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -870,37 +870,37 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SpaceCorgi</t>
+          <t>Nafter</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -910,27 +910,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PlutoPepe</t>
+          <t>Alaska Inu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,27 +940,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kabosu</t>
+          <t>Elongate Deluxe</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -980,17 +980,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MoonTrust</t>
+          <t>SafeZone</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1000,27 +1000,27 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Richie</t>
+          <t>Change Our World</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1030,27 +1030,27 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sanshu Inu</t>
+          <t>Pinknode</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1060,27 +1060,27 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Blocktyme</t>
+          <t>Avalaunch</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1100,7 +1100,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CateCoin</t>
+          <t>SpaceCorgi</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1120,27 +1120,27 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CryptoBlades</t>
+          <t>PlutoPepe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>7 days</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1160,17 +1160,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ShibaPup</t>
+          <t>Kabosu</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1184,23 +1184,23 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Shih Tzu</t>
+          <t>MoonTrust</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1214,83 +1214,83 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Koduro</t>
+          <t>Richie</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ispolink</t>
+          <t>Sanshu Inu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AlgoPainter</t>
+          <t>Blocktyme</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1300,57 +1300,57 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PalGold</t>
+          <t>CateCoin</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2021-05-05</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ganesha Token</t>
+          <t>CryptoBlades</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1360,27 +1360,27 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Pussy Financial</t>
+          <t>ShibaPup</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>10 days</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1390,37 +1390,37 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Gorilla Diamond</t>
+          <t>MoonPirate</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1430,47 +1430,47 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lunar Highway</t>
+          <t>Shih Tzu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CCSwap</t>
+          <t>Koduro</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2021-05-02</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1480,57 +1480,57 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altura</t>
+          <t>Ispolink</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>18 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2021-04-29</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Token Echo</t>
+          <t>AlgoPainter</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>19 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2021-04-28</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1540,71 +1540,281 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BlockBank</t>
+          <t>PalGold</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>19 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2021-04-28</t>
+          <t>2021-05-05</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SafeLaunchpad</t>
+          <t>Oviex</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>21 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2021-04-26</t>
+          <t>2021-05-04</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>2021-05-17</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ganesha Token</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15 days</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2021-05-06</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Pussy Financial</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>15 days</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Gorilla Diamond</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>15 days</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>2021-05-14</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>18</v>
+      <c r="F41" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Lunar Highway</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>15 days</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CCSwap</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2021-05-02</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2021-05-08</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Altura</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19 days</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2021-04-29</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Token Echo</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>20 days</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2021-04-28</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2021-05-08</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Surprise, surprise another update
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,42 +500,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wenlambo</t>
+          <t>Bistroo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5 hours</t>
+          <t xml:space="preserve"> 11 hours</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SafeMusk</t>
+          <t>Wenlambo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -560,12 +560,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YooShi</t>
+          <t>SafeMusk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -590,12 +590,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rune</t>
+          <t>YooShi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -620,12 +620,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tiger King</t>
+          <t>Rune</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -640,22 +640,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GeroWallet</t>
+          <t>Tiger King</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -665,27 +665,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Exohood</t>
+          <t>GeroWallet</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 22 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -700,22 +700,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Relite Finance</t>
+          <t>Exohood</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -740,12 +740,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Convex Finance</t>
+          <t>Relite Finance</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -755,22 +755,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>420x</t>
+          <t>Convex Finance</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -780,32 +780,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EthereumMax</t>
+          <t>420x</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -815,22 +815,22 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Float Protocol: Float</t>
+          <t>Elephant Money</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -840,37 +840,37 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LaunchX</t>
+          <t>EthereumMax</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -884,43 +884,43 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Nafter</t>
+          <t>Wild Ride</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Alaska Inu</t>
+          <t>MoonJuice</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -930,7 +930,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,17 +940,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Elongate Deluxe</t>
+          <t>Float Protocol: Float</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -970,22 +970,22 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SafeZone</t>
+          <t>LaunchX</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1000,22 +1000,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Change Our World</t>
+          <t>Nafter</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1030,17 +1030,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pinknode</t>
+          <t>Alaska Inu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1050,27 +1050,27 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>2021-05-13</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2021-05-15</t>
-        </is>
-      </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Avalaunch</t>
+          <t>Elongate Deluxe</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1080,17 +1080,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>2021-05-13</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1100,17 +1100,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SpaceCorgi</t>
+          <t>SafeZone</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1130,17 +1130,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PlutoPepe</t>
+          <t>Change Our World</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1160,17 +1160,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Kabosu</t>
+          <t>Pinknode</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>6 days</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1180,27 +1180,27 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MoonTrust</t>
+          <t>Avalaunch</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>6 days</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1220,7 +1220,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Richie</t>
+          <t>SpaceCorgi</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1240,17 +1240,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sanshu Inu</t>
+          <t>PlutoPepe</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1274,18 +1274,18 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Blocktyme</t>
+          <t>Kabosu</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1310,12 +1310,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CateCoin</t>
+          <t>MoonTrust</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1340,7 +1340,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CryptoBlades</t>
+          <t>PrivacySwap</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1350,97 +1350,97 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ShibaPup</t>
+          <t>Richie</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>2021-05-10</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>2021-05-08</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2021-05-11</t>
-        </is>
-      </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MoonPirate</t>
+          <t>Sanshu Inu</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Shih Tzu</t>
+          <t>Blocktyme</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1450,27 +1450,27 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Koduro</t>
+          <t>CateCoin</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1480,57 +1480,57 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ispolink</t>
+          <t>CryptoBlades</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>10 days</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AlgoPainter</t>
+          <t>ShibaPup</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>11 days</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1540,27 +1540,27 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PalGold</t>
+          <t>MoonPirate</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>13 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2021-05-05</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1570,57 +1570,57 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Oviex</t>
+          <t>Shih Tzu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ganesha Token</t>
+          <t>Koduro</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1630,57 +1630,57 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Pussy Financial</t>
+          <t>PinkElon</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Gorilla Diamond</t>
+          <t>Ispolink</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -1700,17 +1700,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Lunar Highway</t>
+          <t>AlgoPainter</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1720,27 +1720,27 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CCSwap</t>
+          <t>PalGold</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2021-05-02</t>
+          <t>2021-05-05</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1750,27 +1750,27 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Altura</t>
+          <t>Oviex</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>19 days</t>
+          <t>15 days</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2021-04-29</t>
+          <t>2021-05-04</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1780,41 +1780,221 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Token Echo</t>
+          <t>Ganesha Token</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2021-05-06</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Pussy Financial</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Gorilla Diamond</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Lunar Highway</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Aquari</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2021-05-02</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 day </t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2021-05-18</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CCSwap</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2021-05-02</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2021-05-08</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Altura</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>20 days</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>2021-04-28</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>2021-05-08</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>10</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2021-04-29</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add basic whale tracking info
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,27 +500,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Chihua Token</t>
+          <t>SafeBlast</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 hours</t>
+          <t xml:space="preserve"> 12 hours</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>2021-05-21</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 day </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>2021-05-20</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 day </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -530,27 +530,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Baby Shark</t>
+          <t>CluCoin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 hours</t>
+          <t xml:space="preserve"> 13 hours</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>2021-05-21</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 day </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>2021-05-20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 day </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -560,12 +560,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>American Shiba</t>
+          <t>Chihua Token</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -590,12 +590,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Green Shiba Inu</t>
+          <t>Baby Shark</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 18 hours</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -605,22 +605,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bistroo</t>
+          <t>Chihuahua</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -630,147 +630,147 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>2021-05-20</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 days </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>2021-05-19</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2021-05-17</t>
-        </is>
-      </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Wenlambo</t>
+          <t>American Shiba</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SafeMusk</t>
+          <t>Green Shiba Inu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>2021-05-20</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>2021-05-18</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2021-05-18</t>
-        </is>
-      </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>YooShi</t>
+          <t>Bistroo</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>2021-05-19</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>2021-05-17</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2021-05-18</t>
-        </is>
-      </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Rune</t>
+          <t>Bezoge Earth</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tiger King</t>
+          <t>Wenlambo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -800,7 +800,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GeroWallet</t>
+          <t>SafeMusk</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -824,13 +824,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Exohood</t>
+          <t>YooShi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -860,7 +860,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Relite Finance</t>
+          <t>Rune</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -890,7 +890,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Convex Finance</t>
+          <t>Tiger King</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -900,17 +900,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>2021-05-18</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>2021-05-17</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -920,17 +920,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>420x</t>
+          <t>GeroWallet</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -940,17 +940,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Elephant Money</t>
+          <t>Exohood</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -960,27 +960,27 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EthereumMax</t>
+          <t>Relite Finance</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1004,13 +1004,13 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Wild Ride</t>
+          <t>Convex Finance</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1020,12 +1020,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1034,13 +1034,13 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>upShib</t>
+          <t>420x</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1050,27 +1050,27 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MoonJuice</t>
+          <t>Elephant Money</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1080,27 +1080,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Float Protocol: Float</t>
+          <t>EthereumMax</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1124,23 +1124,23 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LaunchX</t>
+          <t>Wild Ride</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1150,47 +1150,47 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nafter</t>
+          <t>upShib</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Alaska Inu</t>
+          <t>MoonJuice</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1210,17 +1210,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Elongate Deluxe</t>
+          <t>Float Protocol: Float</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1240,17 +1240,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SafeZone</t>
+          <t>LaunchX</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1270,17 +1270,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Change Our World</t>
+          <t>Nafter</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1310,7 +1310,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Pinknode</t>
+          <t>Alaska Inu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1320,27 +1320,27 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>2021-05-13</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2021-05-15</t>
-        </is>
-      </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Avalaunch</t>
+          <t>Elongate Deluxe</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1350,17 +1350,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>2021-05-13</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1370,17 +1370,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SpaceCorgi</t>
+          <t>SafeZone</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>7 days</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1400,17 +1400,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PlutoPepe</t>
+          <t>Change Our World</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>7 days</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1430,47 +1430,47 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SafeOrbit</t>
+          <t>Pinknode</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Kabosu</t>
+          <t>Avalaunch</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1490,17 +1490,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MoonTrust</t>
+          <t>SpaceCorgi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1520,67 +1520,67 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PrivacySwap</t>
+          <t>PlutoPepe</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Richie</t>
+          <t>SafeOrbit</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sanshu Inu</t>
+          <t>Kabosu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1604,13 +1604,13 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Blocktyme</t>
+          <t>MoonTrust</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1630,17 +1630,17 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CateCoin</t>
+          <t>PrivacySwap</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1650,27 +1650,27 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CryptoBlades</t>
+          <t>Richie</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1690,27 +1690,27 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ShibaPup</t>
+          <t>Sanshu Inu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>11 days</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1724,53 +1724,53 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>xxxNifty</t>
+          <t>Blocktyme</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>13 days</t>
+          <t>11 days</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MoonPirate</t>
+          <t>CateCoin</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>11 days</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1780,27 +1780,27 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Shih Tzu</t>
+          <t>CryptoBlades</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1810,27 +1810,27 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Koduro</t>
+          <t>ShibaPup</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1840,17 +1840,17 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PinkElon</t>
+          <t>xxxNifty</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1880,7 +1880,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ispolink</t>
+          <t>MoonPirate</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1904,13 +1904,13 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AlgoPainter</t>
+          <t>Shih Tzu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1930,27 +1930,27 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PalGold</t>
+          <t>Koduro</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2021-05-05</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1960,57 +1960,57 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Oviex</t>
+          <t>PinkElon</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ganesha Token</t>
+          <t>Ispolink</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>15 days</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2020,27 +2020,27 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Pussy Financial</t>
+          <t>AlgoPainter</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>15 days</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2050,27 +2050,27 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Gorilla Diamond</t>
+          <t>PalGold</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>15 days</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2084,23 +2084,23 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Lunar Highway</t>
+          <t>Oviex</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2021-05-03</t>
+          <t>2021-05-05</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2110,71 +2110,161 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>Ganesha Token</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18 days</t>
+          <t>17 days</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2021-05-02</t>
+          <t>2021-05-04</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-06</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CCSwap</t>
+          <t>Pussy Financial</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Gorilla Diamond</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Lunar Highway</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Aquari</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>18 days</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>2021-05-02</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2021-05-08</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
-        <v>6</v>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2021-05-18</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix old whale and total row merge bug
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,27 +500,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SafeBlast</t>
+          <t>ApeHaven</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 12 hours</t>
+          <t xml:space="preserve"> 11 hours</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2021-05-21</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-23</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -530,27 +530,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CluCoin</t>
+          <t>Graviton</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 13 hours</t>
+          <t xml:space="preserve"> 24 hours</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2021-05-21</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-23</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -560,67 +560,67 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chihua Token</t>
+          <t>Orange Token</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t xml:space="preserve"> 24 hours</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Baby Shark</t>
+          <t>NOA PLAY</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t xml:space="preserve"> 24 hours</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chihuahua</t>
+          <t>Netvrk</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -650,17 +650,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>American Shiba</t>
+          <t>SafeBlast</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -670,107 +670,107 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Green Shiba Inu</t>
+          <t>CluCoin</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1 day</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bistroo</t>
+          <t>Chihua Token</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">3 days </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bezoge Earth</t>
+          <t>Baby Shark</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t xml:space="preserve">3 days </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2021-05-21</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Wenlambo</t>
+          <t>Chihuahua</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -790,17 +790,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SafeMusk</t>
+          <t>American Shiba</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -810,17 +810,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">3 days </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-20</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -830,7 +830,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>YooShi</t>
+          <t>Green Shiba Inu</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -840,37 +840,37 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>2021-05-20</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>2021-05-18</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2021-05-18</t>
-        </is>
-      </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rune</t>
+          <t>Bistroo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -880,77 +880,77 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tiger King</t>
+          <t>Bezoge Earth</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GeroWallet</t>
+          <t>Zoo Token</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-23</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Exohood</t>
+          <t>Wenlambo</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -970,27 +970,27 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Relite Finance</t>
+          <t>SafeMusk</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1010,17 +1010,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Convex Finance</t>
+          <t>YooShi</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1034,13 +1034,13 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>420x</t>
+          <t>Rune</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1060,17 +1060,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Elephant Money</t>
+          <t>Tiger King</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1080,27 +1080,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EthereumMax</t>
+          <t>GeroWallet</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1120,17 +1120,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Wild Ride</t>
+          <t>Exohood</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1150,17 +1150,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2021-05-18</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>upShib</t>
+          <t>Relite Finance</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1170,37 +1170,37 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2021-05-16</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MoonJuice</t>
+          <t>Convex Finance</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>5 days</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1220,7 +1220,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Float Protocol: Float</t>
+          <t>420x</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1240,17 +1240,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LaunchX</t>
+          <t>Elephant Money</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1280,17 +1280,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Nafter</t>
+          <t>EthereumMax</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>6 days</t>
+          <t>7 days</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1300,17 +1300,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alaska Inu</t>
+          <t>Wild Ride</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1330,17 +1330,17 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-18</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Elongate Deluxe</t>
+          <t>upShib</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1350,27 +1350,27 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SafeZone</t>
+          <t>Unicly</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1380,27 +1380,27 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">1 day </t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-22</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Change Our World</t>
+          <t>MoonJuice</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1420,27 +1420,27 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pinknode</t>
+          <t>Float Protocol: Float</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8 days</t>
+          <t>7 days</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-16</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1450,17 +1450,17 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Avalaunch</t>
+          <t>LaunchX</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2021-05-13</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1480,27 +1480,27 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SpaceCorgi</t>
+          <t>Nafter</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2021-05-12</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1510,27 +1510,27 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PlutoPepe</t>
+          <t>Alaska Inu</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2021-05-12</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1540,57 +1540,57 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SafeOrbit</t>
+          <t>Elongate Deluxe</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>9 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2021-05-12</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-13</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Kabosu</t>
+          <t>SafeZone</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1600,27 +1600,27 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MoonTrust</t>
+          <t>Change Our World</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>8 days</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1630,57 +1630,57 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PrivacySwap</t>
+          <t>Pinknode</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>10 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2021-05-11</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Richie</t>
+          <t>Avalaunch</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>9 days</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1690,17 +1690,17 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2021-05-08</t>
+          <t>2021-05-14</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sanshu Inu</t>
+          <t>SpaceCorgi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1730,7 +1730,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Blocktyme</t>
+          <t>PlutoPepe</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1760,7 +1760,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CateCoin</t>
+          <t>SafeOrbit</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1770,27 +1770,27 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-05-12</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CryptoBlades</t>
+          <t>Kabosu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1820,7 +1820,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ShibaPup</t>
+          <t>MoonTrust</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2021-05-09</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1844,53 +1844,53 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>xxxNifty</t>
+          <t>PrivacySwap</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 day </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2021-05-20</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MoonPirate</t>
+          <t>Richie</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1900,27 +1900,27 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-08</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Shih Tzu</t>
+          <t>Sanshu Inu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1934,23 +1934,23 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Koduro</t>
+          <t>Blocktyme</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1960,57 +1960,57 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2021-05-15</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PinkElon</t>
+          <t>CateCoin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>12 days</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 days </t>
+          <t>outdated</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2021-05-19</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ispolink</t>
+          <t>CryptoBlades</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>13 days</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2020,27 +2020,27 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2021-05-17</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AlgoPainter</t>
+          <t>ShibaPup</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-09</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2050,47 +2050,47 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>PalGold</t>
+          <t>xxxNifty</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>outdated</t>
+          <t xml:space="preserve">2 days </t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-21</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Oviex</t>
+          <t>MoonPirate</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2021-05-05</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2114,23 +2114,23 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Ganesha Token</t>
+          <t>Shih Tzu</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2140,27 +2140,27 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2021-05-06</t>
+          <t>2021-05-11</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Pussy Financial</t>
+          <t>Koduro</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2170,27 +2170,27 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2021-05-07</t>
+          <t>2021-05-15</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Gorilla Diamond</t>
+          <t>PinkElon</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2200,27 +2200,27 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-19</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Lunar Highway</t>
+          <t>Ispolink</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17 days</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2021-05-04</t>
+          <t>2021-05-07</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2021-05-14</t>
+          <t>2021-05-17</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2240,31 +2240,181 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>AlgoPainter</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>16 days</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2021-05-06</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>PalGold</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>17 days</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2021-05-06</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Oviex</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>18 days</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>2021-05-03</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>outdated</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>2021-05-18</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>15</v>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2021-05-05</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2021-05-17</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Ganesha Token</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>19 days</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2021-05-06</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Pussy Financial</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>19 days</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2021-05-07</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Gorilla Diamond</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>19 days</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2021-05-04</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>outdated</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2021-05-14</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>